<commit_message>
Adding corrections to labs 1-3
</commit_message>
<xml_diff>
--- a/01_hemorrhage/01_hemorrhage_data.xlsx
+++ b/01_hemorrhage/01_hemorrhage_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="9525"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="20730" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -513,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -748,7 +748,7 @@
         <v>72</v>
       </c>
       <c r="C16" s="5">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="D16" s="5">
         <v>83</v>
@@ -778,7 +778,7 @@
         <v>74</v>
       </c>
       <c r="C18" s="5">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="D18" s="5">
         <v>55</v>
@@ -876,7 +876,7 @@
         <v>0.12</v>
       </c>
       <c r="C25" s="5">
-        <v>0.13</v>
+        <v>0.01</v>
       </c>
       <c r="D25" s="5">
         <v>0.01</v>
@@ -958,16 +958,54 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
     <mergeCell ref="F27:F28"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="C22:C24"/>
@@ -979,54 +1017,16 @@
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="E25:E26"/>
     <mergeCell ref="F25:F26"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding change/ Sharing a file over data inconsistancies
</commit_message>
<xml_diff>
--- a/01_hemorrhage/01_hemorrhage_data.xlsx
+++ b/01_hemorrhage/01_hemorrhage_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="31">
   <si>
     <t>Hemorrhage Data</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>HumMod</t>
+  </si>
+  <si>
+    <t>***Cardiac Output is different between the two models</t>
+  </si>
+  <si>
+    <t>***Plasma volume falls again in HumMod for some unknown reason</t>
+  </si>
+  <si>
+    <t>*** The two values differ between QCP and HumMod</t>
   </si>
 </sst>
 </file>
@@ -121,12 +130,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -200,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -229,6 +244,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,13 +539,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29:T29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1">
+    <row r="1" spans="1:21" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -543,7 +561,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:21">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -581,7 +599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1">
+    <row r="3" spans="1:21" ht="15.75" thickBot="1">
       <c r="A3" s="8"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -615,7 +633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:21">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -653,7 +671,7 @@
         <v>5373</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="30.75" thickBot="1">
+    <row r="5" spans="1:21" ht="30.75" thickBot="1">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -671,7 +689,7 @@
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:14" ht="30">
+    <row r="6" spans="1:21" ht="30">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -709,7 +727,7 @@
         <v>2399</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="30.75" thickBot="1">
+    <row r="7" spans="1:21" ht="30.75" thickBot="1">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -727,7 +745,7 @@
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:21">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -765,7 +783,7 @@
         <v>2974</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="30.75" thickBot="1">
+    <row r="9" spans="1:21" ht="30.75" thickBot="1">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -782,8 +800,17 @@
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="O9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -821,7 +848,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1">
+    <row r="11" spans="1:21" ht="15.75" thickBot="1">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -835,7 +862,7 @@
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:21">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -873,7 +900,7 @@
         <v>98.2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="45.75" thickBot="1">
+    <row r="13" spans="1:21" ht="45.75" thickBot="1">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -891,7 +918,7 @@
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="30">
+    <row r="14" spans="1:21" ht="30">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -928,8 +955,16 @@
       <c r="N14" s="7">
         <v>5452</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="45.75" thickBot="1">
+      <c r="O14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+    </row>
+    <row r="15" spans="1:21" ht="45.75" thickBot="1">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
@@ -947,7 +982,7 @@
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:21">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -985,7 +1020,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="30.75" thickBot="1">
+    <row r="17" spans="1:20" ht="30.75" thickBot="1">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -1003,7 +1038,7 @@
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:20">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -1041,7 +1076,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="30.75" thickBot="1">
+    <row r="19" spans="1:20" ht="30.75" thickBot="1">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
@@ -1059,7 +1094,7 @@
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
     </row>
-    <row r="20" spans="1:14" ht="44.25" customHeight="1">
+    <row r="20" spans="1:20" ht="44.25" customHeight="1">
       <c r="A20" s="7" t="s">
         <v>18</v>
       </c>
@@ -1096,8 +1131,16 @@
       <c r="N20" s="7">
         <v>1.51</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1">
+      <c r="O20" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+    </row>
+    <row r="21" spans="1:20" ht="15.75" thickBot="1">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1111,7 +1154,7 @@
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:20">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
@@ -1149,7 +1192,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="30">
+    <row r="23" spans="1:20" ht="30">
       <c r="A23" s="3" t="s">
         <v>19</v>
       </c>
@@ -1166,8 +1209,16 @@
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
-    </row>
-    <row r="24" spans="1:14" ht="30.75" thickBot="1">
+      <c r="O23" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+    </row>
+    <row r="24" spans="1:20" ht="30.75" thickBot="1">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -1185,7 +1236,7 @@
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:20">
       <c r="A25" s="3" t="s">
         <v>21</v>
       </c>
@@ -1222,8 +1273,16 @@
       <c r="N25" s="7">
         <v>0.123</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" ht="45.75" thickBot="1">
+      <c r="O25" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+    </row>
+    <row r="26" spans="1:20" ht="45.75" thickBot="1">
       <c r="A26" s="4" t="s">
         <v>22</v>
       </c>
@@ -1241,7 +1300,7 @@
       <c r="M26" s="8"/>
       <c r="N26" s="8"/>
     </row>
-    <row r="27" spans="1:14" ht="29.25" customHeight="1">
+    <row r="27" spans="1:20" ht="29.25" customHeight="1">
       <c r="A27" s="7" t="s">
         <v>23</v>
       </c>
@@ -1278,8 +1337,16 @@
       <c r="N27" s="7">
         <v>15.8</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" ht="15.75" thickBot="1">
+      <c r="O27" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+    </row>
+    <row r="28" spans="1:20" ht="15.75" thickBot="1">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -1293,7 +1360,7 @@
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
     </row>
-    <row r="29" spans="1:14" ht="30">
+    <row r="29" spans="1:20" ht="30">
       <c r="A29" s="3" t="s">
         <v>24</v>
       </c>
@@ -1330,8 +1397,16 @@
       <c r="N29" s="7">
         <v>801</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" ht="30.75" thickBot="1">
+      <c r="O29" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
+    </row>
+    <row r="30" spans="1:20" ht="30.75" thickBot="1">
       <c r="A30" s="4" t="s">
         <v>25</v>
       </c>
@@ -1351,118 +1426,11 @@
     </row>
   </sheetData>
   <mergeCells count="138">
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="K29:K30"/>
-    <mergeCell ref="L29:L30"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="N29:N30"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="K27:K28"/>
-    <mergeCell ref="L27:L28"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="J22:J24"/>
-    <mergeCell ref="K22:K24"/>
-    <mergeCell ref="L22:L24"/>
-    <mergeCell ref="M22:M24"/>
-    <mergeCell ref="N22:N24"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="C20:C21"/>
@@ -1484,11 +1452,118 @@
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="E27:E28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="K22:K24"/>
+    <mergeCell ref="L22:L24"/>
+    <mergeCell ref="M22:M24"/>
+    <mergeCell ref="N22:N24"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="L29:L30"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="N29:N30"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="M27:M28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixing Lab 1 charts
</commit_message>
<xml_diff>
--- a/01_hemorrhage/01_hemorrhage_data.xlsx
+++ b/01_hemorrhage/01_hemorrhage_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="42">
   <si>
     <t>Hemorrhage Data</t>
   </si>
@@ -112,6 +112,36 @@
   </si>
   <si>
     <t>% Difference</t>
+  </si>
+  <si>
+    <t>Blood Volume</t>
+  </si>
+  <si>
+    <t>Red Cell Volume</t>
+  </si>
+  <si>
+    <t>Plasma Volume</t>
+  </si>
+  <si>
+    <t>Arterial Pressure</t>
+  </si>
+  <si>
+    <t>Cardiac Output</t>
+  </si>
+  <si>
+    <t>Heart Rate</t>
+  </si>
+  <si>
+    <t>Stroke Volume</t>
+  </si>
+  <si>
+    <t>Plasma Renin Act.</t>
+  </si>
+  <si>
+    <t>Na+ Excretion</t>
+  </si>
+  <si>
+    <t>Brain Blood Flow</t>
   </si>
 </sst>
 </file>
@@ -154,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -221,12 +251,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -246,14 +291,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -262,6 +300,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -575,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -596,7 +658,7 @@
       </c>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
@@ -614,7 +676,7 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="J2" s="1">
@@ -634,7 +696,7 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A3" s="12"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -650,7 +712,7 @@
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="12"/>
+      <c r="I3" s="9"/>
       <c r="J3" s="2" t="s">
         <v>2</v>
       </c>
@@ -671,37 +733,37 @@
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="8">
         <v>5413</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="8">
         <v>4420</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="8">
         <v>4465</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="8">
         <v>4724</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="8">
         <v>5531</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="8">
         <v>5421</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="8">
         <v>4432</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="8">
         <v>4554</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="8">
         <v>5053</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="8">
         <v>5373</v>
       </c>
     </row>
@@ -709,55 +771,55 @@
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
       <c r="I5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
     </row>
     <row r="6" spans="1:21" ht="30">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="8">
         <v>2451</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="8">
         <v>1999</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="8">
         <v>1999</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="8">
         <v>2004</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8">
         <v>2426</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="8">
         <v>2340</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="8">
         <v>1909</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="8">
         <v>1909</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="8">
         <v>1916</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="8">
         <v>2399</v>
       </c>
     </row>
@@ -765,55 +827,55 @@
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
       <c r="I7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="8">
         <v>2962</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
         <v>2422</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="8">
         <v>2466</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="8">
         <v>2720</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="8">
         <v>3105</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="8">
         <v>3081</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="8">
         <v>2523</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="8">
         <v>2644</v>
       </c>
-      <c r="M8" s="11">
+      <c r="M8" s="8">
         <v>3137</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="8">
         <v>2974</v>
       </c>
     </row>
@@ -821,116 +883,116 @@
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
       <c r="I9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="9" t="s">
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="8">
         <v>45</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="8">
         <v>45</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="8">
         <v>45</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="8">
         <v>42</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="8">
         <v>44</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="8">
         <v>43</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="8">
         <v>43</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="8">
         <v>42</v>
       </c>
-      <c r="M10" s="11">
+      <c r="M10" s="8">
         <v>38</v>
       </c>
-      <c r="N10" s="11">
+      <c r="N10" s="8">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="8">
         <v>97</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="8">
         <v>79</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="8">
         <v>84</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="8">
         <v>88</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="8">
         <v>98</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="8">
         <v>96.6</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="8">
         <v>94.2</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="8">
         <v>86.5</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="8">
         <v>87.7</v>
       </c>
-      <c r="N12" s="11">
+      <c r="N12" s="8">
         <v>98.2</v>
       </c>
     </row>
@@ -938,119 +1000,119 @@
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
       <c r="I13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
     </row>
     <row r="14" spans="1:21" ht="30">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="8">
         <v>5361</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="8">
         <v>4391</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="8">
         <v>4550</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="8">
         <v>4782</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="8">
         <v>5779</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="8">
         <v>5468</v>
       </c>
-      <c r="K14" s="11">
+      <c r="K14" s="8">
         <v>5763</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L14" s="8">
         <v>5051</v>
       </c>
-      <c r="M14" s="11">
+      <c r="M14" s="8">
         <v>5411</v>
       </c>
-      <c r="N14" s="11">
+      <c r="N14" s="8">
         <v>5452</v>
       </c>
-      <c r="O14" s="9" t="s">
+      <c r="O14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
     </row>
     <row r="15" spans="1:21" ht="45.75" thickBot="1">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
       <c r="I15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="8">
         <v>72</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="8">
         <v>84</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="8">
         <v>83</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="8">
         <v>77</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="8">
         <v>71</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="8">
         <v>72</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="8">
         <v>75</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="8">
         <v>81</v>
       </c>
-      <c r="M16" s="11">
+      <c r="M16" s="8">
         <v>73</v>
       </c>
-      <c r="N16" s="11">
+      <c r="N16" s="8">
         <v>72</v>
       </c>
     </row>
@@ -1058,55 +1120,55 @@
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
       <c r="I17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="8">
         <v>75</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="8">
         <v>52</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="8">
         <v>55</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="8">
         <v>62</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="8">
         <v>81</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="8">
         <v>76</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="8">
         <v>77</v>
       </c>
-      <c r="L18" s="11">
+      <c r="L18" s="8">
         <v>63</v>
       </c>
-      <c r="M18" s="11">
+      <c r="M18" s="8">
         <v>74</v>
       </c>
-      <c r="N18" s="11">
+      <c r="N18" s="8">
         <v>76</v>
       </c>
     </row>
@@ -1114,115 +1176,115 @@
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
       <c r="I19" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
     </row>
     <row r="20" spans="1:20" ht="44.25" customHeight="1">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="8">
         <v>1.5</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="8">
         <v>2.1</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="8">
         <v>1.9</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="8">
         <v>1.7</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="8">
         <v>1.5</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="8">
         <v>1.5</v>
       </c>
-      <c r="K20" s="11">
+      <c r="K20" s="8">
         <v>1.63</v>
       </c>
-      <c r="L20" s="11">
+      <c r="L20" s="8">
         <v>1.85</v>
       </c>
-      <c r="M20" s="11">
+      <c r="M20" s="8">
         <v>1.56</v>
       </c>
-      <c r="N20" s="11">
+      <c r="N20" s="8">
         <v>1.51</v>
       </c>
-      <c r="O20" s="9" t="s">
+      <c r="O20" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
     </row>
     <row r="21" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="8">
         <v>2</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="8">
         <v>2.5</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="8">
         <v>5.5</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="8">
         <v>6</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="8">
         <v>1.7</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J22" s="11">
+      <c r="J22" s="8">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K22" s="11">
+      <c r="K22" s="8">
         <v>2.4</v>
       </c>
-      <c r="L22" s="11">
+      <c r="L22" s="8">
         <v>3.4</v>
       </c>
-      <c r="M22" s="11">
+      <c r="M22" s="8">
         <v>3.4</v>
       </c>
-      <c r="N22" s="11">
+      <c r="N22" s="8">
         <v>2.4</v>
       </c>
     </row>
@@ -1230,858 +1292,789 @@
       <c r="A23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
       <c r="I23" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="9" t="s">
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
     </row>
     <row r="24" spans="1:20" ht="30.75" thickBot="1">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
       <c r="I24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="8">
         <v>0.12</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="8">
         <v>0.01</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="8">
         <v>0.01</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="8">
         <v>0.01</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="8">
         <v>0.14000000000000001</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J25" s="11">
+      <c r="J25" s="8">
         <v>0.123</v>
       </c>
-      <c r="K25" s="11">
+      <c r="K25" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="L25" s="11">
+      <c r="L25" s="8">
         <v>0.03</v>
       </c>
-      <c r="M25" s="11">
+      <c r="M25" s="8">
         <v>2.7E-2</v>
       </c>
-      <c r="N25" s="11">
+      <c r="N25" s="8">
         <v>0.123</v>
       </c>
-      <c r="O25" s="9" t="s">
+      <c r="O25" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
     </row>
     <row r="26" spans="1:20" ht="45.75" thickBot="1">
       <c r="A26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
       <c r="I26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
     </row>
     <row r="27" spans="1:20" ht="29.25" customHeight="1">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27" s="8">
         <v>21</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="8">
         <v>21</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="8">
         <v>23</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="8">
         <v>96</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="8">
         <v>56</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="I27" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J27" s="11">
+      <c r="J27" s="8">
         <v>18.600000000000001</v>
       </c>
-      <c r="K27" s="11">
+      <c r="K27" s="8">
         <v>30.4</v>
       </c>
-      <c r="L27" s="11">
+      <c r="L27" s="8">
         <v>300.5</v>
       </c>
-      <c r="M27" s="11">
+      <c r="M27" s="8">
         <v>118.4</v>
       </c>
-      <c r="N27" s="11">
+      <c r="N27" s="8">
         <v>15.8</v>
       </c>
-      <c r="O27" s="9" t="s">
+      <c r="O27" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
     </row>
     <row r="28" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
     </row>
     <row r="29" spans="1:20" ht="30">
       <c r="A29" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="11">
+      <c r="B29" s="8">
         <v>841</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="8">
         <v>728</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="8">
         <v>781</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="8">
         <v>804</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="8">
         <v>984</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J29" s="11">
+      <c r="J29" s="8">
         <v>796</v>
       </c>
-      <c r="K29" s="11">
+      <c r="K29" s="8">
         <v>934</v>
       </c>
-      <c r="L29" s="11">
+      <c r="L29" s="8">
         <v>830</v>
       </c>
-      <c r="M29" s="11">
+      <c r="M29" s="8">
         <v>816</v>
       </c>
-      <c r="N29" s="11">
+      <c r="N29" s="8">
         <v>801</v>
       </c>
-      <c r="O29" s="9" t="s">
+      <c r="O29" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
     </row>
     <row r="30" spans="1:20" ht="30.75" thickBot="1">
       <c r="A30" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
       <c r="I30" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
     </row>
     <row r="31" spans="1:20" ht="15.75" thickBot="1">
       <c r="B31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" ht="15.75" thickBot="1">
       <c r="B32" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="12">
         <v>0</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="12">
         <v>10</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="12">
         <v>1</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="12">
         <v>1</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B33" s="12"/>
-      <c r="C33" s="2" t="s">
+      <c r="B33" s="11"/>
+      <c r="C33" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="10">
+      <c r="B34" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="13">
         <f>ABS((B4-J4)/B4)</f>
         <v>1.4779235174579716E-3</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="13">
         <f t="shared" ref="D34:G34" si="0">ABS((C4-K4)/C4)</f>
         <v>2.7149321266968325E-3</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="13">
         <f t="shared" si="0"/>
         <v>1.9932810750279955E-2</v>
       </c>
-      <c r="F34" s="10">
+      <c r="F34" s="13">
         <f t="shared" si="0"/>
         <v>6.9644369178662152E-2</v>
       </c>
-      <c r="G34" s="10">
+      <c r="G34" s="13">
         <f t="shared" si="0"/>
         <v>2.8566262881938167E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30.75" thickBot="1">
-      <c r="B35" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-    </row>
-    <row r="36" spans="2:7" ht="30">
-      <c r="B36" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="10">
+    <row r="35" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B35" s="16"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+    </row>
+    <row r="36" spans="2:7" ht="30.75" customHeight="1">
+      <c r="B36" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="13">
         <f t="shared" ref="C36:C59" si="1">ABS((B6-J6)/B6)</f>
         <v>4.528763769889841E-2</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="13">
         <f t="shared" ref="D36:D59" si="2">ABS((C6-K6)/C6)</f>
         <v>4.5022511255627812E-2</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="13">
         <f t="shared" ref="E36:E59" si="3">ABS((D6-L6)/D6)</f>
         <v>4.5022511255627812E-2</v>
       </c>
-      <c r="F36" s="10">
+      <c r="F36" s="13">
         <f t="shared" ref="F36:F59" si="4">ABS((E6-M6)/E6)</f>
         <v>4.3912175648702596E-2</v>
       </c>
-      <c r="G36" s="10">
+      <c r="G36" s="13">
         <f t="shared" ref="G36:G59" si="5">ABS((F6-N6)/F6)</f>
         <v>1.1129431162407255E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30.75" thickBot="1">
-      <c r="B37" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
+    <row r="37" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B37" s="16"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="10">
+      <c r="B38" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="13">
         <f t="shared" si="1"/>
         <v>4.0175557056043212E-2</v>
       </c>
-      <c r="D38" s="10">
+      <c r="D38" s="13">
         <f t="shared" si="2"/>
         <v>4.1701073492981008E-2</v>
       </c>
-      <c r="E38" s="10">
+      <c r="E38" s="13">
         <f t="shared" si="3"/>
         <v>7.2181670721816707E-2</v>
       </c>
-      <c r="F38" s="10">
+      <c r="F38" s="13">
         <f t="shared" si="4"/>
         <v>0.15330882352941178</v>
       </c>
-      <c r="G38" s="10">
+      <c r="G38" s="13">
         <f t="shared" si="5"/>
         <v>4.2190016103059579E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30.75" thickBot="1">
-      <c r="B39" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-    </row>
-    <row r="40" spans="2:7">
+    <row r="39" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B39" s="16"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+    </row>
+    <row r="40" spans="2:7" ht="15.75" thickBot="1">
       <c r="B40" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="13">
         <f t="shared" si="1"/>
         <v>4.4444444444444446E-2</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D40" s="13">
         <f t="shared" si="2"/>
         <v>4.4444444444444446E-2</v>
       </c>
-      <c r="E40" s="10">
+      <c r="E40" s="13">
         <f t="shared" si="3"/>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="F40" s="10">
+      <c r="F40" s="13">
         <f t="shared" si="4"/>
         <v>9.5238095238095233E-2</v>
       </c>
-      <c r="G40" s="10">
+      <c r="G40" s="13">
         <f t="shared" si="5"/>
         <v>2.2727272727272728E-2</v>
       </c>
     </row>
     <row r="41" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B41" s="12"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" s="10">
+      <c r="B42" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="13">
         <f t="shared" si="1"/>
         <v>4.1237113402062438E-3</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D42" s="13">
         <f t="shared" si="2"/>
         <v>0.19240506329113927</v>
       </c>
-      <c r="E42" s="10">
+      <c r="E42" s="13">
         <f t="shared" si="3"/>
         <v>2.976190476190476E-2</v>
       </c>
-      <c r="F42" s="10">
+      <c r="F42" s="13">
         <f t="shared" si="4"/>
         <v>3.4090909090908768E-3</v>
       </c>
-      <c r="G42" s="10">
+      <c r="G42" s="13">
         <f t="shared" si="5"/>
         <v>2.0408163265306411E-3</v>
       </c>
     </row>
-    <row r="43" spans="2:7" ht="45.75" thickBot="1">
-      <c r="B43" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-    </row>
-    <row r="44" spans="2:7" ht="30">
-      <c r="B44" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C44" s="10">
+    <row r="43" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B43" s="16"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+    </row>
+    <row r="44" spans="2:7" ht="30.75" customHeight="1">
+      <c r="B44" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="13">
         <f t="shared" si="1"/>
         <v>1.9958962880059692E-2</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D44" s="13">
         <f t="shared" si="2"/>
         <v>0.31245729902072422</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="13">
         <f t="shared" si="3"/>
         <v>0.11010989010989011</v>
       </c>
-      <c r="F44" s="10">
+      <c r="F44" s="13">
         <f t="shared" si="4"/>
         <v>0.13153492262651612</v>
       </c>
-      <c r="G44" s="10">
+      <c r="G44" s="13">
         <f t="shared" si="5"/>
         <v>5.6584184114898774E-2</v>
       </c>
     </row>
-    <row r="45" spans="2:7" ht="45.75" thickBot="1">
-      <c r="B45" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
+    <row r="45" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B45" s="16"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
     </row>
     <row r="46" spans="2:7">
-      <c r="B46" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C46" s="10">
+      <c r="B46" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D46" s="10">
+      <c r="D46" s="13">
         <f t="shared" si="2"/>
         <v>0.10714285714285714</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E46" s="13">
         <f t="shared" si="3"/>
         <v>2.4096385542168676E-2</v>
       </c>
-      <c r="F46" s="10">
+      <c r="F46" s="13">
         <f t="shared" si="4"/>
         <v>5.1948051948051951E-2</v>
       </c>
-      <c r="G46" s="10">
+      <c r="G46" s="13">
         <f t="shared" si="5"/>
         <v>1.4084507042253521E-2</v>
       </c>
     </row>
-    <row r="47" spans="2:7" ht="30.75" thickBot="1">
-      <c r="B47" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
+    <row r="47" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B47" s="16"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
     </row>
     <row r="48" spans="2:7">
-      <c r="B48" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C48" s="10">
+      <c r="B48" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="13">
         <f t="shared" si="1"/>
         <v>1.3333333333333334E-2</v>
       </c>
-      <c r="D48" s="10">
+      <c r="D48" s="13">
         <f t="shared" si="2"/>
         <v>0.48076923076923078</v>
       </c>
-      <c r="E48" s="10">
+      <c r="E48" s="13">
         <f t="shared" si="3"/>
         <v>0.14545454545454545</v>
       </c>
-      <c r="F48" s="10">
+      <c r="F48" s="13">
         <f t="shared" si="4"/>
         <v>0.19354838709677419</v>
       </c>
-      <c r="G48" s="10">
+      <c r="G48" s="13">
         <f t="shared" si="5"/>
         <v>6.1728395061728392E-2</v>
       </c>
     </row>
-    <row r="49" spans="2:7" ht="30.75" thickBot="1">
-      <c r="B49" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-    </row>
-    <row r="50" spans="2:7">
+    <row r="49" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B49" s="16"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+    </row>
+    <row r="50" spans="2:7" ht="15.75" thickBot="1">
       <c r="B50" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C50" s="10">
+      <c r="C50" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D50" s="10">
+      <c r="D50" s="13">
         <f t="shared" si="2"/>
         <v>0.2238095238095239</v>
       </c>
-      <c r="E50" s="10">
+      <c r="E50" s="13">
         <f t="shared" si="3"/>
         <v>2.6315789473684119E-2</v>
       </c>
-      <c r="F50" s="10">
+      <c r="F50" s="13">
         <f t="shared" si="4"/>
         <v>8.2352941176470532E-2</v>
       </c>
-      <c r="G50" s="10">
+      <c r="G50" s="13">
         <f t="shared" si="5"/>
         <v>6.6666666666666723E-3</v>
       </c>
     </row>
     <row r="51" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B51" s="12"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
     </row>
     <row r="52" spans="2:7">
-      <c r="B52" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" s="10">
+      <c r="B52" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" s="13">
         <f t="shared" si="1"/>
         <v>0.10000000000000009</v>
       </c>
-      <c r="D52" s="10">
+      <c r="D52" s="13">
         <f t="shared" si="2"/>
         <v>4.0000000000000036E-2</v>
       </c>
-      <c r="E52" s="10">
+      <c r="E52" s="13">
         <f t="shared" si="3"/>
         <v>0.38181818181818183</v>
       </c>
-      <c r="F52" s="10">
+      <c r="F52" s="13">
         <f t="shared" si="4"/>
         <v>0.43333333333333335</v>
       </c>
-      <c r="G52" s="10">
+      <c r="G52" s="13">
         <f t="shared" si="5"/>
         <v>0.41176470588235292</v>
       </c>
     </row>
-    <row r="53" spans="2:7" ht="30">
-      <c r="B53" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-    </row>
-    <row r="54" spans="2:7" ht="30.75" thickBot="1">
-      <c r="B54" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
+    <row r="53" spans="2:7">
+      <c r="B53" s="18"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+    </row>
+    <row r="54" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B54" s="16"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
     </row>
     <row r="55" spans="2:7">
-      <c r="B55" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C55" s="10">
+      <c r="B55" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C55" s="13">
         <f t="shared" si="1"/>
         <v>2.5000000000000022E-2</v>
       </c>
-      <c r="D55" s="10">
+      <c r="D55" s="13">
         <f>ABS((C25-K25)/C25)</f>
         <v>13</v>
       </c>
-      <c r="E55" s="10">
+      <c r="E55" s="13">
         <f t="shared" si="3"/>
         <v>1.9999999999999996</v>
       </c>
-      <c r="F55" s="10">
+      <c r="F55" s="13">
         <f t="shared" si="4"/>
         <v>1.7000000000000002</v>
       </c>
-      <c r="G55" s="10">
+      <c r="G55" s="13">
         <f t="shared" si="5"/>
         <v>0.12142857142857152</v>
       </c>
     </row>
-    <row r="56" spans="2:7" ht="45.75" thickBot="1">
-      <c r="B56" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
-    </row>
-    <row r="57" spans="2:7">
+    <row r="56" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B56" s="16"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+    </row>
+    <row r="57" spans="2:7" ht="15.75" thickBot="1">
       <c r="B57" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C57" s="10">
+      <c r="C57" s="13">
         <f t="shared" si="1"/>
         <v>0.11428571428571421</v>
       </c>
-      <c r="D57" s="10">
+      <c r="D57" s="13">
         <f t="shared" si="2"/>
         <v>0.44761904761904753</v>
       </c>
-      <c r="E57" s="10">
+      <c r="E57" s="13">
         <f t="shared" si="3"/>
         <v>12.065217391304348</v>
       </c>
-      <c r="F57" s="10">
+      <c r="F57" s="13">
         <f t="shared" si="4"/>
         <v>0.23333333333333339</v>
       </c>
-      <c r="G57" s="10">
+      <c r="G57" s="13">
         <f t="shared" si="5"/>
         <v>0.71785714285714286</v>
       </c>
     </row>
     <row r="58" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B58" s="12"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10"/>
-    </row>
-    <row r="59" spans="2:7" ht="30">
-      <c r="B59" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C59" s="10">
+      <c r="B58" s="11"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+    </row>
+    <row r="59" spans="2:7" ht="30.75" customHeight="1">
+      <c r="B59" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C59" s="13">
         <f t="shared" si="1"/>
         <v>5.3507728894173601E-2</v>
       </c>
-      <c r="D59" s="10">
+      <c r="D59" s="13">
         <f t="shared" si="2"/>
         <v>0.28296703296703296</v>
       </c>
-      <c r="E59" s="10">
+      <c r="E59" s="13">
         <f t="shared" si="3"/>
         <v>6.2740076824583865E-2</v>
       </c>
-      <c r="F59" s="10">
+      <c r="F59" s="13">
         <f t="shared" si="4"/>
         <v>1.4925373134328358E-2</v>
       </c>
-      <c r="G59" s="10">
+      <c r="G59" s="13">
         <f t="shared" si="5"/>
         <v>0.18597560975609756</v>
       </c>
     </row>
-    <row r="60" spans="2:7" ht="30.75" thickBot="1">
-      <c r="B60" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="10"/>
+    <row r="60" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B60" s="16"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="142">
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="J22:J24"/>
-    <mergeCell ref="K22:K24"/>
-    <mergeCell ref="L22:L24"/>
-    <mergeCell ref="M22:M24"/>
-    <mergeCell ref="N22:N24"/>
+  <mergeCells count="217">
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="G52:G54"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="B50:B51"/>
@@ -2104,8 +2097,130 @@
     <mergeCell ref="D29:D30"/>
     <mergeCell ref="E29:E30"/>
     <mergeCell ref="F29:F30"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="K22:K24"/>
+    <mergeCell ref="L22:L24"/>
+    <mergeCell ref="M22:M24"/>
+    <mergeCell ref="N22:N24"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
   </mergeCells>
-  <conditionalFormatting sqref="C34:G60">
+  <conditionalFormatting sqref="C34:G52 D55:G60 C55 C57:C60">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>